<commit_message>
Level2 Report Partially Implemented
</commit_message>
<xml_diff>
--- a/api-server-django/api/assessment/sample/level1.xlsx
+++ b/api-server-django/api/assessment/sample/level1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Freelancing\Paraclete\api-server-django\api\assessment\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BDC367-242B-4D6A-9C36-A2A477324D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67554661-7902-4600-8901-EDB410BF23E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page1" sheetId="9" r:id="rId1"/>
@@ -1132,6 +1132,45 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1147,9 +1186,6 @@
     <xf numFmtId="0" fontId="14" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1159,42 +1195,6 @@
     <xf numFmtId="0" fontId="30" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1234,26 +1234,41 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1275,21 +1290,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3365,7 +3365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD9BE586-3C54-41A9-80C8-C44D336AB6A8}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="47" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="47" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
@@ -3974,7 +3974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7288371C-FBD6-46BE-A8A0-B55AC3B5E822}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D42" sqref="D42:G44"/>
     </sheetView>
   </sheetViews>
@@ -4166,11 +4166,11 @@
       <c r="A14" s="73"/>
       <c r="B14" s="74"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="101" t="s">
+      <c r="D14" s="113" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="101"/>
-      <c r="F14" s="101"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="113"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
@@ -4182,11 +4182,11 @@
         <v>49</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="102" t="s">
+      <c r="D15" s="114" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="102"/>
-      <c r="F15" s="102"/>
+      <c r="E15" s="114"/>
+      <c r="F15" s="114"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
@@ -4194,9 +4194,9 @@
       <c r="A16" s="73"/>
       <c r="B16" s="74"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="102"/>
-      <c r="E16" s="102"/>
-      <c r="F16" s="102"/>
+      <c r="D16" s="114"/>
+      <c r="E16" s="114"/>
+      <c r="F16" s="114"/>
       <c r="G16" s="5"/>
       <c r="H16" s="20"/>
     </row>
@@ -4256,7 +4256,7 @@
       <c r="A21" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="94" t="s">
+      <c r="B21" s="107" t="s">
         <v>54</v>
       </c>
       <c r="C21" s="5"/>
@@ -4268,7 +4268,7 @@
     </row>
     <row r="22" spans="1:10" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="73"/>
-      <c r="B22" s="94"/>
+      <c r="B22" s="107"/>
       <c r="C22" s="5"/>
       <c r="D22" s="31"/>
       <c r="E22" s="31"/>
@@ -4278,7 +4278,7 @@
     </row>
     <row r="23" spans="1:10" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="73"/>
-      <c r="B23" s="94"/>
+      <c r="B23" s="107"/>
       <c r="C23" s="5"/>
       <c r="D23" s="49" t="s">
         <v>24</v>
@@ -4290,7 +4290,7 @@
     </row>
     <row r="24" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="73"/>
-      <c r="B24" s="94"/>
+      <c r="B24" s="107"/>
       <c r="C24" s="5"/>
       <c r="D24" s="84" t="s">
         <v>3</v>
@@ -4305,7 +4305,7 @@
     </row>
     <row r="25" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="73"/>
-      <c r="B25" s="94"/>
+      <c r="B25" s="107"/>
       <c r="C25" s="5"/>
       <c r="D25" s="84"/>
       <c r="E25" s="84"/>
@@ -4377,12 +4377,12 @@
         <v>59</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="95" t="s">
+      <c r="D30" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="96"/>
-      <c r="F30" s="96"/>
-      <c r="G30" s="97"/>
+      <c r="E30" s="109"/>
+      <c r="F30" s="109"/>
+      <c r="G30" s="110"/>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4393,103 +4393,103 @@
         <v>60</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="98"/>
-      <c r="E31" s="99"/>
-      <c r="F31" s="99"/>
-      <c r="G31" s="100"/>
+      <c r="D31" s="111"/>
+      <c r="E31" s="98"/>
+      <c r="F31" s="98"/>
+      <c r="G31" s="112"/>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="73"/>
       <c r="B32" s="74"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="107" t="s">
+      <c r="D32" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="108"/>
-      <c r="F32" s="108"/>
-      <c r="G32" s="109"/>
+      <c r="E32" s="95"/>
+      <c r="F32" s="95"/>
+      <c r="G32" s="96"/>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="94" t="s">
+      <c r="B33" s="107" t="s">
         <v>62</v>
       </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="110"/>
-      <c r="E33" s="99"/>
-      <c r="F33" s="99"/>
-      <c r="G33" s="111"/>
+      <c r="D33" s="97"/>
+      <c r="E33" s="98"/>
+      <c r="F33" s="98"/>
+      <c r="G33" s="99"/>
       <c r="H33" s="5"/>
       <c r="R33" s="2"/>
     </row>
     <row r="34" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="73"/>
-      <c r="B34" s="94"/>
+      <c r="B34" s="107"/>
       <c r="C34" s="5"/>
-      <c r="D34" s="107" t="s">
+      <c r="D34" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="E34" s="108"/>
-      <c r="F34" s="108"/>
-      <c r="G34" s="109"/>
+      <c r="E34" s="95"/>
+      <c r="F34" s="95"/>
+      <c r="G34" s="96"/>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:18" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="73"/>
-      <c r="B35" s="94"/>
+      <c r="B35" s="107"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="110"/>
-      <c r="E35" s="99"/>
-      <c r="F35" s="99"/>
-      <c r="G35" s="111"/>
+      <c r="D35" s="97"/>
+      <c r="E35" s="98"/>
+      <c r="F35" s="98"/>
+      <c r="G35" s="99"/>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="78"/>
       <c r="B36" s="79"/>
       <c r="C36" s="5"/>
-      <c r="D36" s="107" t="s">
+      <c r="D36" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="108"/>
-      <c r="F36" s="108"/>
-      <c r="G36" s="109"/>
+      <c r="E36" s="95"/>
+      <c r="F36" s="95"/>
+      <c r="G36" s="96"/>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="71"/>
       <c r="B37" s="72"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="110"/>
-      <c r="E37" s="99"/>
-      <c r="F37" s="99"/>
-      <c r="G37" s="111"/>
+      <c r="D37" s="97"/>
+      <c r="E37" s="98"/>
+      <c r="F37" s="98"/>
+      <c r="G37" s="99"/>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="71"/>
       <c r="B38" s="72"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="107" t="s">
+      <c r="D38" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="108"/>
-      <c r="F38" s="108"/>
-      <c r="G38" s="109"/>
+      <c r="E38" s="95"/>
+      <c r="F38" s="95"/>
+      <c r="G38" s="96"/>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="71"/>
       <c r="B39" s="72"/>
       <c r="C39" s="5"/>
-      <c r="D39" s="110"/>
-      <c r="E39" s="99"/>
-      <c r="F39" s="99"/>
-      <c r="G39" s="111"/>
+      <c r="D39" s="97"/>
+      <c r="E39" s="98"/>
+      <c r="F39" s="98"/>
+      <c r="G39" s="99"/>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -4506,11 +4506,11 @@
       <c r="A41" s="71"/>
       <c r="B41" s="72"/>
       <c r="C41" s="5"/>
-      <c r="D41" s="114" t="s">
+      <c r="D41" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="E41" s="114"/>
-      <c r="F41" s="114"/>
+      <c r="E41" s="102"/>
+      <c r="F41" s="102"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
@@ -4554,12 +4554,12 @@
       <c r="A45" s="71"/>
       <c r="B45" s="72"/>
       <c r="C45" s="5"/>
-      <c r="D45" s="113" t="s">
+      <c r="D45" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="E45" s="113"/>
-      <c r="F45" s="113"/>
-      <c r="G45" s="113"/>
+      <c r="E45" s="101"/>
+      <c r="F45" s="101"/>
+      <c r="G45" s="101"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
     </row>
@@ -4567,12 +4567,12 @@
       <c r="A46" s="71"/>
       <c r="B46" s="72"/>
       <c r="C46" s="5"/>
-      <c r="D46" s="112" t="s">
+      <c r="D46" s="100" t="s">
         <v>63</v>
       </c>
-      <c r="E46" s="112"/>
-      <c r="F46" s="112"/>
-      <c r="G46" s="112"/>
+      <c r="E46" s="100"/>
+      <c r="F46" s="100"/>
+      <c r="G46" s="100"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
     </row>
@@ -4580,10 +4580,10 @@
       <c r="A47" s="71"/>
       <c r="B47" s="72"/>
       <c r="C47" s="5"/>
-      <c r="D47" s="112"/>
-      <c r="E47" s="112"/>
-      <c r="F47" s="112"/>
-      <c r="G47" s="112"/>
+      <c r="D47" s="100"/>
+      <c r="E47" s="100"/>
+      <c r="F47" s="100"/>
+      <c r="G47" s="100"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
     </row>
@@ -4591,10 +4591,10 @@
       <c r="A48" s="71"/>
       <c r="B48" s="72"/>
       <c r="C48" s="5"/>
-      <c r="D48" s="112"/>
-      <c r="E48" s="112"/>
-      <c r="F48" s="112"/>
-      <c r="G48" s="112"/>
+      <c r="D48" s="100"/>
+      <c r="E48" s="100"/>
+      <c r="F48" s="100"/>
+      <c r="G48" s="100"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
     </row>
@@ -4602,10 +4602,10 @@
       <c r="A49" s="71"/>
       <c r="B49" s="72"/>
       <c r="C49" s="5"/>
-      <c r="D49" s="112"/>
-      <c r="E49" s="112"/>
-      <c r="F49" s="112"/>
-      <c r="G49" s="112"/>
+      <c r="D49" s="100"/>
+      <c r="E49" s="100"/>
+      <c r="F49" s="100"/>
+      <c r="G49" s="100"/>
       <c r="H49" s="5"/>
     </row>
     <row r="50" spans="1:8" ht="8.5500000000000007" customHeight="1" x14ac:dyDescent="0.25">
@@ -4667,6 +4667,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="D24:G25"/>
+    <mergeCell ref="D30:G31"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F16"/>
+    <mergeCell ref="D8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D19:G21"/>
     <mergeCell ref="A53:H53"/>
     <mergeCell ref="E52:F52"/>
     <mergeCell ref="D38:G39"/>
@@ -4677,17 +4688,6 @@
     <mergeCell ref="D45:G45"/>
     <mergeCell ref="D41:F41"/>
     <mergeCell ref="D42:G44"/>
-    <mergeCell ref="D8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D19:G21"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="D24:G25"/>
-    <mergeCell ref="D30:G31"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F16"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4951,13 +4951,13 @@
     </row>
     <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="95" t="s">
+      <c r="B21" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="96"/>
-      <c r="D21" s="96"/>
-      <c r="E21" s="96"/>
-      <c r="F21" s="96"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="109"/>
+      <c r="E21" s="109"/>
+      <c r="F21" s="109"/>
       <c r="G21" s="62"/>
       <c r="H21" s="5"/>
     </row>
@@ -4973,14 +4973,14 @@
     </row>
     <row r="23" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
-      <c r="B23" s="95" t="s">
+      <c r="B23" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="96"/>
-      <c r="F23" s="96"/>
-      <c r="G23" s="97"/>
+      <c r="C23" s="109"/>
+      <c r="D23" s="109"/>
+      <c r="E23" s="109"/>
+      <c r="F23" s="109"/>
+      <c r="G23" s="110"/>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5146,56 +5146,56 @@
     </row>
     <row r="39" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
-      <c r="B39" s="113" t="s">
+      <c r="B39" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="113"/>
-      <c r="D39" s="113"/>
-      <c r="E39" s="113"/>
-      <c r="F39" s="113"/>
-      <c r="G39" s="113"/>
+      <c r="C39" s="101"/>
+      <c r="D39" s="101"/>
+      <c r="E39" s="101"/>
+      <c r="F39" s="101"/>
+      <c r="G39" s="101"/>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
-      <c r="B40" s="112" t="s">
+      <c r="B40" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="C40" s="112"/>
-      <c r="D40" s="112"/>
-      <c r="E40" s="112"/>
-      <c r="F40" s="112"/>
-      <c r="G40" s="112"/>
+      <c r="C40" s="100"/>
+      <c r="D40" s="100"/>
+      <c r="E40" s="100"/>
+      <c r="F40" s="100"/>
+      <c r="G40" s="100"/>
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
-      <c r="B41" s="112"/>
-      <c r="C41" s="112"/>
-      <c r="D41" s="112"/>
-      <c r="E41" s="112"/>
-      <c r="F41" s="112"/>
-      <c r="G41" s="112"/>
+      <c r="B41" s="100"/>
+      <c r="C41" s="100"/>
+      <c r="D41" s="100"/>
+      <c r="E41" s="100"/>
+      <c r="F41" s="100"/>
+      <c r="G41" s="100"/>
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
-      <c r="B42" s="112"/>
-      <c r="C42" s="112"/>
-      <c r="D42" s="112"/>
-      <c r="E42" s="112"/>
-      <c r="F42" s="112"/>
-      <c r="G42" s="112"/>
+      <c r="B42" s="100"/>
+      <c r="C42" s="100"/>
+      <c r="D42" s="100"/>
+      <c r="E42" s="100"/>
+      <c r="F42" s="100"/>
+      <c r="G42" s="100"/>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
-      <c r="B43" s="112"/>
-      <c r="C43" s="112"/>
-      <c r="D43" s="112"/>
-      <c r="E43" s="112"/>
-      <c r="F43" s="112"/>
-      <c r="G43" s="112"/>
+      <c r="B43" s="100"/>
+      <c r="C43" s="100"/>
+      <c r="D43" s="100"/>
+      <c r="E43" s="100"/>
+      <c r="F43" s="100"/>
+      <c r="G43" s="100"/>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -5595,13 +5595,13 @@
     </row>
     <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="95" t="s">
+      <c r="B21" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="96"/>
-      <c r="D21" s="96"/>
-      <c r="E21" s="96"/>
-      <c r="F21" s="96"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="109"/>
+      <c r="E21" s="109"/>
+      <c r="F21" s="109"/>
       <c r="G21" s="62"/>
       <c r="H21" s="5"/>
     </row>
@@ -5617,14 +5617,14 @@
     </row>
     <row r="23" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
-      <c r="B23" s="95" t="s">
+      <c r="B23" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="96"/>
-      <c r="F23" s="96"/>
-      <c r="G23" s="97"/>
+      <c r="C23" s="109"/>
+      <c r="D23" s="109"/>
+      <c r="E23" s="109"/>
+      <c r="F23" s="109"/>
+      <c r="G23" s="110"/>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5790,56 +5790,56 @@
     </row>
     <row r="39" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
-      <c r="B39" s="113" t="s">
+      <c r="B39" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="113"/>
-      <c r="D39" s="113"/>
-      <c r="E39" s="113"/>
-      <c r="F39" s="113"/>
-      <c r="G39" s="113"/>
+      <c r="C39" s="101"/>
+      <c r="D39" s="101"/>
+      <c r="E39" s="101"/>
+      <c r="F39" s="101"/>
+      <c r="G39" s="101"/>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
-      <c r="B40" s="112" t="s">
+      <c r="B40" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="112"/>
-      <c r="D40" s="112"/>
-      <c r="E40" s="112"/>
-      <c r="F40" s="112"/>
-      <c r="G40" s="112"/>
+      <c r="C40" s="100"/>
+      <c r="D40" s="100"/>
+      <c r="E40" s="100"/>
+      <c r="F40" s="100"/>
+      <c r="G40" s="100"/>
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
-      <c r="B41" s="112"/>
-      <c r="C41" s="112"/>
-      <c r="D41" s="112"/>
-      <c r="E41" s="112"/>
-      <c r="F41" s="112"/>
-      <c r="G41" s="112"/>
+      <c r="B41" s="100"/>
+      <c r="C41" s="100"/>
+      <c r="D41" s="100"/>
+      <c r="E41" s="100"/>
+      <c r="F41" s="100"/>
+      <c r="G41" s="100"/>
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
-      <c r="B42" s="112"/>
-      <c r="C42" s="112"/>
-      <c r="D42" s="112"/>
-      <c r="E42" s="112"/>
-      <c r="F42" s="112"/>
-      <c r="G42" s="112"/>
+      <c r="B42" s="100"/>
+      <c r="C42" s="100"/>
+      <c r="D42" s="100"/>
+      <c r="E42" s="100"/>
+      <c r="F42" s="100"/>
+      <c r="G42" s="100"/>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
-      <c r="B43" s="112"/>
-      <c r="C43" s="112"/>
-      <c r="D43" s="112"/>
-      <c r="E43" s="112"/>
-      <c r="F43" s="112"/>
-      <c r="G43" s="112"/>
+      <c r="B43" s="100"/>
+      <c r="C43" s="100"/>
+      <c r="D43" s="100"/>
+      <c r="E43" s="100"/>
+      <c r="F43" s="100"/>
+      <c r="G43" s="100"/>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -5988,7 +5988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F842EA94-A732-4734-AB0F-54444B0B1E8B}">
   <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B42" sqref="B42:G49"/>
     </sheetView>
   </sheetViews>
@@ -6074,52 +6074,52 @@
     </row>
     <row r="7" spans="1:8" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="131" t="s">
+      <c r="B7" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="131"/>
-      <c r="D7" s="131"/>
-      <c r="E7" s="131"/>
+      <c r="C7" s="128"/>
+      <c r="D7" s="128"/>
+      <c r="E7" s="128"/>
       <c r="F7" s="30"/>
       <c r="G7" s="30"/>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="131"/>
-      <c r="C8" s="131"/>
-      <c r="D8" s="131"/>
-      <c r="E8" s="131"/>
+      <c r="B8" s="128"/>
+      <c r="C8" s="128"/>
+      <c r="D8" s="128"/>
+      <c r="E8" s="128"/>
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="131"/>
-      <c r="E9" s="131"/>
+      <c r="B9" s="128"/>
+      <c r="C9" s="128"/>
+      <c r="D9" s="128"/>
+      <c r="E9" s="128"/>
       <c r="F9" s="5"/>
       <c r="G9" s="14"/>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="131"/>
-      <c r="C10" s="131"/>
-      <c r="D10" s="131"/>
-      <c r="E10" s="131"/>
+      <c r="B10" s="128"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="128"/>
+      <c r="E10" s="128"/>
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="131"/>
-      <c r="C11" s="131"/>
-      <c r="D11" s="131"/>
-      <c r="E11" s="131"/>
+      <c r="B11" s="128"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="128"/>
+      <c r="E11" s="128"/>
       <c r="F11" s="24"/>
       <c r="G11" s="24"/>
       <c r="H11" s="5"/>
@@ -6146,11 +6146,11 @@
     </row>
     <row r="14" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
-      <c r="B14" s="134" t="s">
+      <c r="B14" s="133" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="134"/>
-      <c r="D14" s="134"/>
+      <c r="C14" s="133"/>
+      <c r="D14" s="133"/>
       <c r="E14" s="24"/>
       <c r="F14" s="24"/>
       <c r="G14" s="24"/>
@@ -6193,11 +6193,11 @@
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
       <c r="D18" s="32"/>
-      <c r="E18" s="134" t="s">
+      <c r="E18" s="133" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="134"/>
-      <c r="G18" s="134"/>
+      <c r="F18" s="133"/>
+      <c r="G18" s="133"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:19" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -6238,11 +6238,11 @@
     </row>
     <row r="21" spans="1:19" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
-      <c r="B21" s="134" t="s">
+      <c r="B21" s="133" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="134"/>
-      <c r="D21" s="134"/>
+      <c r="C21" s="133"/>
+      <c r="D21" s="133"/>
       <c r="E21" s="129"/>
       <c r="F21" s="129"/>
       <c r="G21" s="129"/>
@@ -6327,14 +6327,14 @@
     </row>
     <row r="26" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
-      <c r="B26" s="132" t="s">
+      <c r="B26" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="132"/>
-      <c r="D26" s="132"/>
-      <c r="E26" s="132"/>
-      <c r="F26" s="132"/>
-      <c r="G26" s="132"/>
+      <c r="C26" s="130"/>
+      <c r="D26" s="130"/>
+      <c r="E26" s="130"/>
+      <c r="F26" s="130"/>
+      <c r="G26" s="130"/>
       <c r="H26" s="5"/>
       <c r="M26"/>
       <c r="N26"/>
@@ -6437,14 +6437,14 @@
     </row>
     <row r="32" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
-      <c r="B32" s="133" t="s">
+      <c r="B32" s="131" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="133"/>
-      <c r="D32" s="133"/>
-      <c r="E32" s="133"/>
-      <c r="F32" s="133"/>
-      <c r="G32" s="133"/>
+      <c r="C32" s="131"/>
+      <c r="D32" s="131"/>
+      <c r="E32" s="131"/>
+      <c r="F32" s="131"/>
+      <c r="G32" s="131"/>
       <c r="H32" s="5"/>
       <c r="M32"/>
       <c r="N32"/>
@@ -6456,12 +6456,12 @@
     </row>
     <row r="33" spans="1:19" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
-      <c r="B33" s="133"/>
-      <c r="C33" s="133"/>
-      <c r="D33" s="133"/>
-      <c r="E33" s="133"/>
-      <c r="F33" s="133"/>
-      <c r="G33" s="133"/>
+      <c r="B33" s="131"/>
+      <c r="C33" s="131"/>
+      <c r="D33" s="131"/>
+      <c r="E33" s="131"/>
+      <c r="F33" s="131"/>
+      <c r="G33" s="131"/>
       <c r="H33" s="5"/>
       <c r="M33"/>
       <c r="N33"/>
@@ -6507,14 +6507,14 @@
     </row>
     <row r="36" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
-      <c r="B36" s="130" t="s">
+      <c r="B36" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="130"/>
-      <c r="D36" s="130"/>
-      <c r="E36" s="130"/>
-      <c r="F36" s="130"/>
-      <c r="G36" s="130"/>
+      <c r="C36" s="132"/>
+      <c r="D36" s="132"/>
+      <c r="E36" s="132"/>
+      <c r="F36" s="132"/>
+      <c r="G36" s="132"/>
       <c r="H36" s="5"/>
       <c r="M36"/>
       <c r="N36"/>
@@ -6545,14 +6545,14 @@
     </row>
     <row r="38" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
-      <c r="B38" s="130">
+      <c r="B38" s="132">
         <v>2</v>
       </c>
-      <c r="C38" s="130"/>
-      <c r="D38" s="130"/>
-      <c r="E38" s="130"/>
-      <c r="F38" s="130"/>
-      <c r="G38" s="130"/>
+      <c r="C38" s="132"/>
+      <c r="D38" s="132"/>
+      <c r="E38" s="132"/>
+      <c r="F38" s="132"/>
+      <c r="G38" s="132"/>
       <c r="H38" s="5"/>
       <c r="M38"/>
       <c r="N38"/>
@@ -6564,14 +6564,14 @@
     </row>
     <row r="39" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
-      <c r="B39" s="130">
+      <c r="B39" s="132">
         <v>3</v>
       </c>
-      <c r="C39" s="130"/>
-      <c r="D39" s="130"/>
-      <c r="E39" s="130"/>
-      <c r="F39" s="130"/>
-      <c r="G39" s="130"/>
+      <c r="C39" s="132"/>
+      <c r="D39" s="132"/>
+      <c r="E39" s="132"/>
+      <c r="F39" s="132"/>
+      <c r="G39" s="132"/>
       <c r="H39" s="5"/>
       <c r="M39"/>
       <c r="N39"/>
@@ -6617,14 +6617,14 @@
     </row>
     <row r="42" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
-      <c r="B42" s="128" t="s">
+      <c r="B42" s="134" t="s">
         <v>66</v>
       </c>
-      <c r="C42" s="128"/>
-      <c r="D42" s="128"/>
-      <c r="E42" s="128"/>
-      <c r="F42" s="128"/>
-      <c r="G42" s="128"/>
+      <c r="C42" s="134"/>
+      <c r="D42" s="134"/>
+      <c r="E42" s="134"/>
+      <c r="F42" s="134"/>
+      <c r="G42" s="134"/>
       <c r="H42" s="5"/>
       <c r="M42"/>
       <c r="N42"/>
@@ -6636,12 +6636,12 @@
     </row>
     <row r="43" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
-      <c r="B43" s="128"/>
-      <c r="C43" s="128"/>
-      <c r="D43" s="128"/>
-      <c r="E43" s="128"/>
-      <c r="F43" s="128"/>
-      <c r="G43" s="128"/>
+      <c r="B43" s="134"/>
+      <c r="C43" s="134"/>
+      <c r="D43" s="134"/>
+      <c r="E43" s="134"/>
+      <c r="F43" s="134"/>
+      <c r="G43" s="134"/>
       <c r="H43" s="5"/>
       <c r="M43"/>
       <c r="N43"/>
@@ -6653,12 +6653,12 @@
     </row>
     <row r="44" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
-      <c r="B44" s="128"/>
-      <c r="C44" s="128"/>
-      <c r="D44" s="128"/>
-      <c r="E44" s="128"/>
-      <c r="F44" s="128"/>
-      <c r="G44" s="128"/>
+      <c r="B44" s="134"/>
+      <c r="C44" s="134"/>
+      <c r="D44" s="134"/>
+      <c r="E44" s="134"/>
+      <c r="F44" s="134"/>
+      <c r="G44" s="134"/>
       <c r="H44" s="5"/>
       <c r="M44"/>
       <c r="N44"/>
@@ -6670,12 +6670,12 @@
     </row>
     <row r="45" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
-      <c r="B45" s="128"/>
-      <c r="C45" s="128"/>
-      <c r="D45" s="128"/>
-      <c r="E45" s="128"/>
-      <c r="F45" s="128"/>
-      <c r="G45" s="128"/>
+      <c r="B45" s="134"/>
+      <c r="C45" s="134"/>
+      <c r="D45" s="134"/>
+      <c r="E45" s="134"/>
+      <c r="F45" s="134"/>
+      <c r="G45" s="134"/>
       <c r="H45" s="5"/>
       <c r="M45"/>
       <c r="N45"/>
@@ -6687,12 +6687,12 @@
     </row>
     <row r="46" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
-      <c r="B46" s="128"/>
-      <c r="C46" s="128"/>
-      <c r="D46" s="128"/>
-      <c r="E46" s="128"/>
-      <c r="F46" s="128"/>
-      <c r="G46" s="128"/>
+      <c r="B46" s="134"/>
+      <c r="C46" s="134"/>
+      <c r="D46" s="134"/>
+      <c r="E46" s="134"/>
+      <c r="F46" s="134"/>
+      <c r="G46" s="134"/>
       <c r="H46" s="5"/>
       <c r="M46"/>
       <c r="N46"/>
@@ -6704,12 +6704,12 @@
     </row>
     <row r="47" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
-      <c r="B47" s="128"/>
-      <c r="C47" s="128"/>
-      <c r="D47" s="128"/>
-      <c r="E47" s="128"/>
-      <c r="F47" s="128"/>
-      <c r="G47" s="128"/>
+      <c r="B47" s="134"/>
+      <c r="C47" s="134"/>
+      <c r="D47" s="134"/>
+      <c r="E47" s="134"/>
+      <c r="F47" s="134"/>
+      <c r="G47" s="134"/>
       <c r="H47" s="5"/>
       <c r="M47"/>
       <c r="N47"/>
@@ -6721,12 +6721,12 @@
     </row>
     <row r="48" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
-      <c r="B48" s="128"/>
-      <c r="C48" s="128"/>
-      <c r="D48" s="128"/>
-      <c r="E48" s="128"/>
-      <c r="F48" s="128"/>
-      <c r="G48" s="128"/>
+      <c r="B48" s="134"/>
+      <c r="C48" s="134"/>
+      <c r="D48" s="134"/>
+      <c r="E48" s="134"/>
+      <c r="F48" s="134"/>
+      <c r="G48" s="134"/>
       <c r="H48" s="5"/>
       <c r="M48"/>
       <c r="N48"/>
@@ -6738,12 +6738,12 @@
     </row>
     <row r="49" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
-      <c r="B49" s="128"/>
-      <c r="C49" s="128"/>
-      <c r="D49" s="128"/>
-      <c r="E49" s="128"/>
-      <c r="F49" s="128"/>
-      <c r="G49" s="128"/>
+      <c r="B49" s="134"/>
+      <c r="C49" s="134"/>
+      <c r="D49" s="134"/>
+      <c r="E49" s="134"/>
+      <c r="F49" s="134"/>
+      <c r="G49" s="134"/>
       <c r="H49" s="5"/>
       <c r="M49"/>
       <c r="N49"/>
@@ -6819,6 +6819,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A53:H53"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="B42:G49"/>
+    <mergeCell ref="B22:E24"/>
+    <mergeCell ref="B15:E17"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B39:G39"/>
     <mergeCell ref="B7:E11"/>
     <mergeCell ref="E19:G21"/>
     <mergeCell ref="B26:G26"/>
@@ -6827,13 +6834,6 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="B21:D21"/>
-    <mergeCell ref="A53:H53"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="B42:G49"/>
-    <mergeCell ref="B22:E24"/>
-    <mergeCell ref="B15:E17"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B39:G39"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -6932,12 +6932,12 @@
     </row>
     <row r="7" spans="1:8" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="131" t="s">
+      <c r="B7" s="128" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="131"/>
-      <c r="D7" s="131"/>
-      <c r="E7" s="131"/>
+      <c r="C7" s="128"/>
+      <c r="D7" s="128"/>
+      <c r="E7" s="128"/>
       <c r="F7" s="30"/>
       <c r="G7" s="30"/>
       <c r="H7" s="5"/>
@@ -6954,24 +6954,24 @@
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="137" t="s">
+      <c r="B9" s="142" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="137"/>
-      <c r="D9" s="137"/>
-      <c r="E9" s="137"/>
-      <c r="F9" s="137"/>
-      <c r="G9" s="137"/>
+      <c r="C9" s="142"/>
+      <c r="D9" s="142"/>
+      <c r="E9" s="142"/>
+      <c r="F9" s="142"/>
+      <c r="G9" s="142"/>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="137"/>
-      <c r="C10" s="137"/>
-      <c r="D10" s="137"/>
-      <c r="E10" s="137"/>
-      <c r="F10" s="137"/>
-      <c r="G10" s="137"/>
+      <c r="B10" s="142"/>
+      <c r="C10" s="142"/>
+      <c r="D10" s="142"/>
+      <c r="E10" s="142"/>
+      <c r="F10" s="142"/>
+      <c r="G10" s="142"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -7003,8 +7003,8 @@
       <c r="B13" s="24"/>
       <c r="C13" s="84"/>
       <c r="D13" s="84"/>
-      <c r="E13" s="138"/>
-      <c r="F13" s="138"/>
+      <c r="E13" s="143"/>
+      <c r="F13" s="143"/>
       <c r="G13" s="19"/>
       <c r="H13" s="5"/>
     </row>
@@ -7013,16 +7013,16 @@
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
       <c r="D14" s="24"/>
-      <c r="E14" s="138"/>
-      <c r="F14" s="138"/>
+      <c r="E14" s="143"/>
+      <c r="F14" s="143"/>
       <c r="G14" s="24"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="19"/>
-      <c r="C15" s="142"/>
-      <c r="D15" s="142"/>
+      <c r="C15" s="139"/>
+      <c r="D15" s="139"/>
       <c r="E15" s="84"/>
       <c r="F15" s="84"/>
       <c r="G15" s="19"/>
@@ -7080,16 +7080,16 @@
     </row>
     <row r="21" spans="1:18" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
-      <c r="B21" s="139" t="s">
+      <c r="B21" s="144" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="140"/>
-      <c r="D21" s="141"/>
+      <c r="C21" s="145"/>
+      <c r="D21" s="146"/>
       <c r="E21" s="19"/>
-      <c r="F21" s="139" t="s">
+      <c r="F21" s="144" t="s">
         <v>32</v>
       </c>
-      <c r="G21" s="141"/>
+      <c r="G21" s="146"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7105,8 +7105,8 @@
     <row r="23" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="19"/>
       <c r="B23" s="54"/>
-      <c r="C23" s="143"/>
-      <c r="D23" s="144"/>
+      <c r="C23" s="135"/>
+      <c r="D23" s="136"/>
       <c r="E23" s="19"/>
       <c r="F23" s="42"/>
       <c r="G23" s="44"/>
@@ -7115,8 +7115,8 @@
     <row r="24" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="19"/>
       <c r="B24" s="54"/>
-      <c r="C24" s="143"/>
-      <c r="D24" s="144"/>
+      <c r="C24" s="135"/>
+      <c r="D24" s="136"/>
       <c r="E24" s="19"/>
       <c r="F24" s="42"/>
       <c r="G24" s="44"/>
@@ -7125,8 +7125,8 @@
     <row r="25" spans="1:18" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="55"/>
-      <c r="C25" s="145"/>
-      <c r="D25" s="146"/>
+      <c r="C25" s="137"/>
+      <c r="D25" s="138"/>
       <c r="E25" s="41"/>
       <c r="F25" s="43"/>
       <c r="G25" s="45"/>
@@ -7137,8 +7137,8 @@
       <c r="B26" s="24"/>
       <c r="C26" s="84"/>
       <c r="D26" s="84"/>
-      <c r="E26" s="138"/>
-      <c r="F26" s="138"/>
+      <c r="E26" s="143"/>
+      <c r="F26" s="143"/>
       <c r="G26" s="19"/>
       <c r="H26" s="5"/>
     </row>
@@ -7147,16 +7147,16 @@
       <c r="B27" s="24"/>
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
-      <c r="E27" s="138"/>
-      <c r="F27" s="138"/>
+      <c r="E27" s="143"/>
+      <c r="F27" s="143"/>
       <c r="G27" s="24"/>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="19"/>
-      <c r="C28" s="142"/>
-      <c r="D28" s="142"/>
+      <c r="C28" s="139"/>
+      <c r="D28" s="139"/>
       <c r="E28" s="24"/>
       <c r="F28" s="32"/>
       <c r="G28" s="19"/>
@@ -7335,46 +7335,46 @@
     </row>
     <row r="46" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
-      <c r="B46" s="135" t="s">
+      <c r="B46" s="140" t="s">
         <v>19</v>
       </c>
-      <c r="C46" s="135"/>
-      <c r="D46" s="135"/>
-      <c r="E46" s="135"/>
-      <c r="F46" s="135"/>
-      <c r="G46" s="135"/>
+      <c r="C46" s="140"/>
+      <c r="D46" s="140"/>
+      <c r="E46" s="140"/>
+      <c r="F46" s="140"/>
+      <c r="G46" s="140"/>
       <c r="H46" s="5"/>
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
-      <c r="B47" s="135"/>
-      <c r="C47" s="135"/>
-      <c r="D47" s="135"/>
-      <c r="E47" s="135"/>
-      <c r="F47" s="135"/>
-      <c r="G47" s="135"/>
+      <c r="B47" s="140"/>
+      <c r="C47" s="140"/>
+      <c r="D47" s="140"/>
+      <c r="E47" s="140"/>
+      <c r="F47" s="140"/>
+      <c r="G47" s="140"/>
       <c r="H47" s="5"/>
     </row>
     <row r="48" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
-      <c r="B48" s="136" t="s">
+      <c r="B48" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="C48" s="136"/>
-      <c r="D48" s="136"/>
-      <c r="E48" s="136"/>
-      <c r="F48" s="136"/>
-      <c r="G48" s="136"/>
+      <c r="C48" s="141"/>
+      <c r="D48" s="141"/>
+      <c r="E48" s="141"/>
+      <c r="F48" s="141"/>
+      <c r="G48" s="141"/>
       <c r="H48" s="5"/>
     </row>
     <row r="49" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
-      <c r="B49" s="136"/>
-      <c r="C49" s="136"/>
-      <c r="D49" s="136"/>
-      <c r="E49" s="136"/>
-      <c r="F49" s="136"/>
-      <c r="G49" s="136"/>
+      <c r="B49" s="141"/>
+      <c r="C49" s="141"/>
+      <c r="D49" s="141"/>
+      <c r="E49" s="141"/>
+      <c r="F49" s="141"/>
+      <c r="G49" s="141"/>
       <c r="H49" s="5"/>
     </row>
     <row r="50" spans="1:8" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -7436,11 +7436,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="B46:G47"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="A53:H53"/>
     <mergeCell ref="B7:E7"/>
@@ -7456,6 +7451,11 @@
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="E26:F27"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="B46:G47"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>